<commit_message>
Added functionality to update files
</commit_message>
<xml_diff>
--- a/JS/1000.xlsx
+++ b/JS/1000.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">OS</t>
   </si>
   <si>
-    <t xml:space="preserve">Windows 10</t>
+    <t xml:space="preserve">Ubuntu</t>
   </si>
   <si>
     <t xml:space="preserve">Price </t>
@@ -191,10 +191,10 @@
   <dimension ref="C1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.37"/>
   </cols>
@@ -228,7 +228,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>300</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>